<commit_message>
fix labels in concepts for legal, tech
- fixes missing whitespace in labels ("like so")
- thanks to @JonathanBowker for fixes
- resolves #76
- resolves #77
- resolves #78
- resolves #79
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/dpv-tech.xlsx
+++ b/documentation-generator/vocab_csv/dpv-tech.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="266">
   <si>
     <t>Term</t>
   </si>
@@ -172,6 +172,9 @@
     <t>TechnologyActor</t>
   </si>
   <si>
+    <t>Technology Actor</t>
+  </si>
+  <si>
     <t>Actors and Entities involved in provision, use, and management of Technology</t>
   </si>
   <si>
@@ -181,6 +184,9 @@
     <t>TechnologyUsageLocation</t>
   </si>
   <si>
+    <t>Technology Usage Location</t>
+  </si>
+  <si>
     <t>Location for where technology is provided or used</t>
   </si>
   <si>
@@ -190,12 +196,18 @@
     <t>CommunicationMechanism</t>
   </si>
   <si>
+    <t>Communication Mechanism</t>
+  </si>
+  <si>
     <t>Communication mechanism used or provided by Technologoy</t>
   </si>
   <si>
     <t>TechnologyReadinessLevel</t>
   </si>
   <si>
+    <t>Technology Readiness Level</t>
+  </si>
+  <si>
     <t>Indication of maturity of Technology (ISO 16290:2013)</t>
   </si>
   <si>
@@ -505,6 +517,9 @@
     <t>FixedUse</t>
   </si>
   <si>
+    <t>Fixed Use</t>
+  </si>
+  <si>
     <t>Technology that can be used a fixed numner of times</t>
   </si>
   <si>
@@ -562,6 +577,9 @@
     <t>hasProvisionMethod</t>
   </si>
   <si>
+    <t>has provision method</t>
+  </si>
+  <si>
     <t>Specifies the provision or usage method of technology</t>
   </si>
   <si>
@@ -571,30 +589,45 @@
     <t>TechnologyProvider</t>
   </si>
   <si>
+    <t>Technology Provider</t>
+  </si>
+  <si>
     <t>Actor that provides Technology</t>
   </si>
   <si>
     <t>TechnologyDeveloper</t>
   </si>
   <si>
+    <t>Technology Developer</t>
+  </si>
+  <si>
     <t>Actor that develops Technology</t>
   </si>
   <si>
     <t>TechnologyUser</t>
   </si>
   <si>
+    <t>Technology User</t>
+  </si>
+  <si>
     <t>Actor that uses Technologoy</t>
   </si>
   <si>
     <t>TechnologySubject</t>
   </si>
   <si>
+    <t>Technology Subject</t>
+  </si>
+  <si>
     <t>Actor that is subject of use of Technology</t>
   </si>
   <si>
     <t>hasProvider</t>
   </si>
   <si>
+    <t>has provider</t>
+  </si>
+  <si>
     <t>Indicates technology provider</t>
   </si>
   <si>
@@ -607,6 +640,9 @@
     <t>hasDeveloper</t>
   </si>
   <si>
+    <t>has developer</t>
+  </si>
+  <si>
     <t>Indicates technology developer</t>
   </si>
   <si>
@@ -616,6 +652,9 @@
     <t>hasUser</t>
   </si>
   <si>
+    <t>has user</t>
+  </si>
+  <si>
     <t>Indicates technology user</t>
   </si>
   <si>
@@ -625,6 +664,9 @@
     <t>hasSubject</t>
   </si>
   <si>
+    <t>has subject</t>
+  </si>
+  <si>
     <t>Indicates technology subject</t>
   </si>
   <si>
@@ -643,6 +685,9 @@
     <t>LocalNetwork</t>
   </si>
   <si>
+    <t>Local Network</t>
+  </si>
+  <si>
     <t>Technology utilising local networking communication</t>
   </si>
   <si>
@@ -670,6 +715,9 @@
     <t>CellularNetwork</t>
   </si>
   <si>
+    <t>Cellular Network</t>
+  </si>
+  <si>
     <t>Technology utilising cellular networking communication</t>
   </si>
   <si>
@@ -703,12 +751,18 @@
     <t>FileSystem</t>
   </si>
   <si>
+    <t>File System</t>
+  </si>
+  <si>
     <t>A data storage and retrieval interface provided by an operating system</t>
   </si>
   <si>
     <t>SmartphoneApplication</t>
   </si>
   <si>
+    <t>Smartphone Application</t>
+  </si>
+  <si>
     <t>A computing or digital program on a smartphone device</t>
   </si>
   <si>
@@ -718,6 +772,9 @@
     <t>PersonalInformationManagementSystem</t>
   </si>
   <si>
+    <t>Personal Information Management System</t>
+  </si>
+  <si>
     <t>A PIMS is a system that helps to give individuals more control over their personal data by managing their personal data in secure, on-premises or online storage systems and sharing it when and with whomever they choose</t>
   </si>
   <si>
@@ -727,6 +784,9 @@
     <t>IdentityManagementTechnology</t>
   </si>
   <si>
+    <t>Identity Management Technology</t>
+  </si>
+  <si>
     <t>Technologies providing identity provision, verification, management, and governance</t>
   </si>
   <si>
@@ -734,6 +794,9 @@
   </si>
   <si>
     <t>IdentityWallet</t>
+  </si>
+  <si>
+    <t>Identity Wallet</t>
   </si>
   <si>
     <t xml:space="preserve">product and service that allows the user to store identity data, credentials and attributes linked to her/his identity, to provide them to relying parties on request and to use them for authentication, online and offline, and to create qualified electronic signatures and seals </t>
@@ -929,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -990,7 +1053,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -1006,9 +1069,6 @@
     </xf>
     <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -1808,13 +1868,13 @@
         <v>48</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>26</v>
@@ -1855,16 +1915,16 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>26</v>
@@ -1905,13 +1965,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>18</v>
@@ -1955,13 +2015,13 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>16</v>
@@ -2068,13 +2128,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
@@ -2089,7 +2149,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>11</v>
@@ -2106,22 +2166,22 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
@@ -2134,7 +2194,7 @@
         <v>44855.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>28</v>
@@ -2158,22 +2218,22 @@
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
@@ -2186,7 +2246,7 @@
         <v>44855.0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N3" s="25" t="s">
         <v>28</v>
@@ -2210,22 +2270,22 @@
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
@@ -2238,7 +2298,7 @@
         <v>44855.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N4" s="25" t="s">
         <v>28</v>
@@ -2262,22 +2322,22 @@
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>199</v>
+        <v>212</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>213</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
@@ -2290,7 +2350,7 @@
         <v>44855.0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>28</v>
@@ -2342,7 +2402,7 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B17" s="6"/>
     </row>
@@ -2461,10 +2521,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2473,22 +2533,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -2529,16 +2589,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -2579,16 +2639,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -2629,16 +2689,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -2679,16 +2739,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -2729,16 +2789,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -2779,16 +2839,16 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>26</v>
@@ -2930,28 +2990,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>218</v>
+      <c r="A2" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>234</v>
       </c>
       <c r="C2" s="19"/>
-      <c r="D2" s="29"/>
+      <c r="D2" s="28"/>
       <c r="K2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>221</v>
+      <c r="A3" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>237</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -2991,17 +3051,17 @@
       <c r="AD3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="30" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>222</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>224</v>
+      <c r="A4" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>240</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -3041,17 +3101,17 @@
       <c r="AD4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>221</v>
+      <c r="A5" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>237</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -3091,17 +3151,17 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>229</v>
+      <c r="A6" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>247</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -3141,17 +3201,17 @@
       <c r="AD6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>232</v>
+      <c r="A7" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -3191,17 +3251,17 @@
       <c r="AD7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>235</v>
+      <c r="A8" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>255</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -3241,17 +3301,17 @@
       <c r="AD8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>238</v>
+      <c r="A9" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>259</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -3394,27 +3454,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="J2" s="34" t="s">
-        <v>240</v>
+      <c r="J2" s="33" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>242</v>
+        <v>262</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>244</v>
+        <v>264</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="6">
@@ -3739,59 +3799,59 @@
       <c r="K79" s="8"/>
     </row>
     <row r="80">
-      <c r="A80" s="28"/>
-      <c r="B80" s="28"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="19"/>
-      <c r="D80" s="29"/>
+      <c r="D80" s="28"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="31"/>
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="30"/>
       <c r="K81" s="8"/>
     </row>
     <row r="82">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="31"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="30"/>
       <c r="K82" s="8"/>
     </row>
     <row r="83">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="31"/>
+      <c r="A83" s="29"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="30"/>
       <c r="K83" s="8"/>
     </row>
     <row r="84">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="31"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="30"/>
       <c r="K84" s="8"/>
     </row>
     <row r="85">
-      <c r="A85" s="32"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="31"/>
+      <c r="A85" s="31"/>
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="30"/>
       <c r="K85" s="8"/>
     </row>
     <row r="86">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="33"/>
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="32"/>
       <c r="K86" s="8"/>
     </row>
     <row r="87">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="31"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="30"/>
       <c r="K87" s="8"/>
     </row>
   </sheetData>
@@ -3866,13 +3926,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
@@ -3887,7 +3947,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>11</v>
@@ -3904,19 +3964,19 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>21</v>
@@ -3930,7 +3990,7 @@
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>28</v>
@@ -3954,19 +4014,19 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>21</v>
@@ -3980,7 +4040,7 @@
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>28</v>
@@ -4004,19 +4064,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>21</v>
@@ -4075,7 +4135,7 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B15" s="6"/>
     </row>
@@ -4227,26 +4287,26 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -4287,16 +4347,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -4337,16 +4397,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -4387,16 +4447,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -4437,16 +4497,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -4487,16 +4547,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -4537,16 +4597,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -4587,16 +4647,16 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>26</v>
@@ -4637,16 +4697,16 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>26</v>
@@ -4687,16 +4747,16 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>26</v>
@@ -4737,16 +4797,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>26</v>
@@ -4893,10 +4953,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="17"/>
@@ -4905,16 +4965,16 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -4955,16 +5015,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5005,16 +5065,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>121</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>117</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -5055,16 +5115,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -5204,10 +5264,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -5238,16 +5298,16 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -5265,7 +5325,7 @@
         <v>27</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>29</v>
@@ -5288,16 +5348,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5315,7 +5375,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>29</v>
@@ -5338,16 +5398,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -5365,7 +5425,7 @@
         <v>27</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>29</v>
@@ -5388,16 +5448,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -5415,7 +5475,7 @@
         <v>27</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>29</v>
@@ -5438,16 +5498,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -5465,7 +5525,7 @@
         <v>27</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>29</v>
@@ -5488,16 +5548,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -5515,7 +5575,7 @@
         <v>27</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>29</v>
@@ -5639,25 +5699,25 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="K2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -5666,7 +5726,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="8">
@@ -5700,16 +5760,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5718,7 +5778,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="8">
@@ -5849,10 +5909,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -5867,19 +5927,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -5917,19 +5977,19 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -5967,19 +6027,19 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6017,19 +6077,19 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -6067,25 +6127,25 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="8">
@@ -6093,7 +6153,7 @@
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>28</v>
@@ -6117,19 +6177,19 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -6167,19 +6227,19 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -6217,19 +6277,19 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -6327,13 +6387,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
@@ -6348,7 +6408,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>11</v>
@@ -6365,19 +6425,19 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>21</v>
@@ -6391,7 +6451,7 @@
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>28</v>
@@ -6443,7 +6503,7 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B14" s="6"/>
     </row>
@@ -6564,10 +6624,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -6582,16 +6642,16 @@
     </row>
     <row r="4">
       <c r="A4" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>181</v>
+        <v>187</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -6632,16 +6692,16 @@
     </row>
     <row r="5">
       <c r="A5" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>191</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -6682,16 +6742,16 @@
     </row>
     <row r="6">
       <c r="A6" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>185</v>
+        <v>193</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -6732,16 +6792,16 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>187</v>
+        <v>196</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
resolves #49 GDPR legal basis to rights mapping
The mappings are added using dpv:hasRight to legal basis module in
DPV-GDPR, and are rendered in a separate section in HTML listing the
applicable rights for each legal basis.
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/dpv-tech.xlsx
+++ b/documentation-generator/vocab_csv/dpv-tech.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="294">
   <si>
     <t>Term</t>
   </si>
@@ -376,6 +376,21 @@
     <t>dpv-tech:DataTechnology,dpv-tech:ManagementTechnology</t>
   </si>
   <si>
+    <t>DataIntermediationTechnology</t>
+  </si>
+  <si>
+    <t>Data Intermediation Technology</t>
+  </si>
+  <si>
+    <t>Technology related to the provision of data intermediation services</t>
+  </si>
+  <si>
+    <t>DGA 10.a</t>
+  </si>
+  <si>
+    <t>proposed</t>
+  </si>
+  <si>
     <t>Operations / Processing Technologies</t>
   </si>
   <si>
@@ -620,6 +635,75 @@
   </si>
   <si>
     <t>Actor that is subject of use of Technology</t>
+  </si>
+  <si>
+    <t>TechnologyDesigner</t>
+  </si>
+  <si>
+    <t>Technology Designer</t>
+  </si>
+  <si>
+    <t>Actor that designs Technology</t>
+  </si>
+  <si>
+    <t>tech:TechnologyActor</t>
+  </si>
+  <si>
+    <t>DGA 26.3</t>
+  </si>
+  <si>
+    <t>TechnologyInstaller</t>
+  </si>
+  <si>
+    <t>Technology Installer</t>
+  </si>
+  <si>
+    <t>Actor that installs Technology</t>
+  </si>
+  <si>
+    <t>TechnologyMaintainer</t>
+  </si>
+  <si>
+    <t>Technology Maintainer</t>
+  </si>
+  <si>
+    <t>Actor that maintains Technology</t>
+  </si>
+  <si>
+    <t>TechnologyManufacturer</t>
+  </si>
+  <si>
+    <t>Technology Manufacturer</t>
+  </si>
+  <si>
+    <t>Actor that manufactures Technology</t>
+  </si>
+  <si>
+    <t>TechnologyOwner</t>
+  </si>
+  <si>
+    <t>Technology Owner</t>
+  </si>
+  <si>
+    <t>Actor that owns Technology</t>
+  </si>
+  <si>
+    <t>TechnologyPurchaser</t>
+  </si>
+  <si>
+    <t>Technology Purchaser</t>
+  </si>
+  <si>
+    <t>Actor that purchases Technology</t>
+  </si>
+  <si>
+    <t>TechnologySupplier</t>
+  </si>
+  <si>
+    <t>Technology Supplier</t>
+  </si>
+  <si>
+    <t>Actor that supplies Technology</t>
   </si>
   <si>
     <t>hasProvider</t>
@@ -860,7 +944,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -891,6 +975,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -992,7 +1081,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1043,52 +1132,64 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2165,28 +2266,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>201</v>
+      <c r="A2" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>229</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>202</v>
+      <c r="E2" s="27" t="s">
+        <v>230</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+        <v>231</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="24"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="8">
         <v>44744.0</v>
       </c>
@@ -2196,49 +2297,49 @@
       <c r="M2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>206</v>
+      <c r="A3" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>234</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>207</v>
+      <c r="E3" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+        <v>231</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="24"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="8">
         <v>44744.0</v>
       </c>
@@ -2248,49 +2349,49 @@
       <c r="M3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>210</v>
+      <c r="A4" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>238</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>211</v>
+      <c r="E4" s="27" t="s">
+        <v>239</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+        <v>231</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="24"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="8">
         <v>44744.0</v>
       </c>
@@ -2300,49 +2401,49 @@
       <c r="M4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
     </row>
     <row r="5">
-      <c r="A5" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>214</v>
+      <c r="A5" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>242</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>215</v>
+      <c r="E5" s="27" t="s">
+        <v>243</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+        <v>231</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="24"/>
+      <c r="J5" s="28"/>
       <c r="K5" s="8">
         <v>44744.0</v>
       </c>
@@ -2352,25 +2453,25 @@
       <c r="M5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="O5" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
     </row>
     <row r="6">
       <c r="B6" s="16"/>
@@ -2521,10 +2622,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2539,13 +2640,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>69</v>
@@ -2589,16 +2690,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -2639,16 +2740,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -2689,16 +2790,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -2739,16 +2840,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -2789,16 +2890,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>229</v>
+        <v>257</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>230</v>
+        <v>258</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -2839,13 +2940,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>69</v>
@@ -2990,28 +3091,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="28"/>
+      <c r="A2" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="32"/>
       <c r="K2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>237</v>
+      <c r="A3" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>265</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -3051,17 +3152,17 @@
       <c r="AD3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>240</v>
+      <c r="A4" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>268</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -3101,17 +3202,17 @@
       <c r="AD4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>237</v>
+      <c r="A5" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>265</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -3151,17 +3252,17 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>247</v>
+      <c r="A6" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>275</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -3201,17 +3302,17 @@
       <c r="AD6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>251</v>
+      <c r="A7" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>279</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -3251,17 +3352,17 @@
       <c r="AD7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>254</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>255</v>
+      <c r="A8" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>283</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -3301,17 +3402,17 @@
       <c r="AD8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>259</v>
+      <c r="A9" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>287</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -3454,27 +3555,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="J2" s="33" t="s">
-        <v>261</v>
+      <c r="J2" s="37" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>263</v>
+        <v>290</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>265</v>
+        <v>292</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="6">
@@ -3563,23 +3664,23 @@
     <row r="27">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="21"/>
       <c r="K27" s="8"/>
     </row>
     <row r="28">
-      <c r="D28" s="17"/>
+      <c r="D28" s="21"/>
       <c r="K28" s="8"/>
     </row>
     <row r="29">
-      <c r="D29" s="17"/>
+      <c r="D29" s="21"/>
       <c r="K29" s="8"/>
     </row>
     <row r="30">
-      <c r="D30" s="17"/>
+      <c r="D30" s="21"/>
       <c r="K30" s="8"/>
     </row>
     <row r="31">
-      <c r="D31" s="17"/>
+      <c r="D31" s="21"/>
       <c r="K31" s="8"/>
     </row>
     <row r="32">
@@ -3590,30 +3691,30 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="18"/>
+      <c r="L33" s="22"/>
       <c r="M33" s="5"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="18"/>
-      <c r="Y33" s="18"/>
-      <c r="Z33" s="18"/>
-      <c r="AA33" s="18"/>
-      <c r="AB33" s="18"/>
-      <c r="AC33" s="18"/>
-      <c r="AD33" s="18"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
     </row>
     <row r="34">
       <c r="K34" s="8"/>
@@ -3694,23 +3795,23 @@
       <c r="K57" s="8"/>
     </row>
     <row r="58">
-      <c r="A58" s="19"/>
-      <c r="B58" s="19"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
       <c r="K58" s="8"/>
     </row>
     <row r="59">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
       <c r="K59" s="8"/>
     </row>
     <row r="60">
-      <c r="A60" s="19"/>
-      <c r="B60" s="19"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
       <c r="K60" s="8"/>
     </row>
     <row r="61">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
       <c r="K61" s="8"/>
     </row>
     <row r="62">
@@ -3767,30 +3868,30 @@
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
       <c r="K77" s="8"/>
-      <c r="L77" s="18"/>
+      <c r="L77" s="22"/>
       <c r="M77" s="5"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="18"/>
-      <c r="T77" s="18"/>
-      <c r="U77" s="18"/>
-      <c r="V77" s="18"/>
-      <c r="W77" s="18"/>
-      <c r="X77" s="18"/>
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="18"/>
-      <c r="AA77" s="18"/>
-      <c r="AB77" s="18"/>
-      <c r="AC77" s="18"/>
-      <c r="AD77" s="18"/>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
+      <c r="R77" s="22"/>
+      <c r="S77" s="22"/>
+      <c r="T77" s="22"/>
+      <c r="U77" s="22"/>
+      <c r="V77" s="22"/>
+      <c r="W77" s="22"/>
+      <c r="X77" s="22"/>
+      <c r="Y77" s="22"/>
+      <c r="Z77" s="22"/>
+      <c r="AA77" s="22"/>
+      <c r="AB77" s="22"/>
+      <c r="AC77" s="22"/>
+      <c r="AD77" s="22"/>
     </row>
     <row r="78">
       <c r="K78" s="8"/>
@@ -3799,59 +3900,59 @@
       <c r="K79" s="8"/>
     </row>
     <row r="80">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="28"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="32"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81">
-      <c r="A81" s="29"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="30"/>
+      <c r="A81" s="33"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="34"/>
       <c r="K81" s="8"/>
     </row>
     <row r="82">
-      <c r="A82" s="29"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="30"/>
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="34"/>
       <c r="K82" s="8"/>
     </row>
     <row r="83">
-      <c r="A83" s="29"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="30"/>
+      <c r="A83" s="33"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="34"/>
       <c r="K83" s="8"/>
     </row>
     <row r="84">
-      <c r="A84" s="29"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="30"/>
+      <c r="A84" s="33"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="34"/>
       <c r="K84" s="8"/>
     </row>
     <row r="85">
-      <c r="A85" s="31"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="30"/>
+      <c r="A85" s="35"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="34"/>
       <c r="K85" s="8"/>
     </row>
     <row r="86">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="32"/>
+      <c r="A86" s="33"/>
+      <c r="B86" s="33"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="36"/>
       <c r="K86" s="8"/>
     </row>
     <row r="87">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="30"/>
+      <c r="A87" s="33"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="34"/>
       <c r="K87" s="8"/>
     </row>
   </sheetData>
@@ -4344,6 +4445,7 @@
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
@@ -4394,6 +4496,7 @@
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
@@ -4444,6 +4547,7 @@
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
@@ -4494,6 +4598,7 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
@@ -4544,6 +4649,7 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
@@ -4594,6 +4700,7 @@
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
@@ -4644,6 +4751,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
@@ -4694,6 +4802,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -4744,6 +4853,7 @@
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
@@ -4794,6 +4904,7 @@
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
@@ -4844,9 +4955,55 @@
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AD150">
+  <conditionalFormatting sqref="A2:AE150">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
@@ -4861,7 +5018,7 @@
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O150 AC2:AD150 K4 K7 K10 A13:L150 P13:AB150">
+  <conditionalFormatting sqref="M2:O150 AC2:AE150 K4 K7 K10 A13:L150 P13:AB150">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
@@ -4953,28 +5110,28 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="17"/>
+      <c r="D2" s="21"/>
       <c r="K2" s="8"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -5015,16 +5172,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>121</v>
+        <v>129</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5065,16 +5222,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>126</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>121</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -5115,16 +5272,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -5264,50 +5421,50 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="18"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="5"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -5325,7 +5482,7 @@
         <v>27</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>29</v>
@@ -5348,16 +5505,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5375,7 +5532,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>29</v>
@@ -5398,16 +5555,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
@@ -5425,7 +5582,7 @@
         <v>27</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>29</v>
@@ -5448,16 +5605,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -5475,7 +5632,7 @@
         <v>27</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>29</v>
@@ -5498,16 +5655,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -5525,7 +5682,7 @@
         <v>27</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>29</v>
@@ -5548,16 +5705,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -5575,7 +5732,7 @@
         <v>27</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>29</v>
@@ -5699,25 +5856,25 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="K2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
@@ -5726,7 +5883,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="8">
@@ -5760,16 +5917,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -5778,7 +5935,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="8">
@@ -5909,10 +6066,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -5927,19 +6084,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -5977,19 +6134,19 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -6027,19 +6184,19 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6077,19 +6234,19 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -6127,25 +6284,25 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="8">
@@ -6177,19 +6334,19 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -6227,19 +6384,19 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -6277,19 +6434,19 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -6425,19 +6582,19 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>21</v>
@@ -6624,10 +6781,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -6641,14 +6798,14 @@
       <c r="K3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
-        <v>187</v>
+      <c r="A4" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>78</v>
@@ -6689,16 +6846,17 @@
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
-        <v>190</v>
+      <c r="A5" s="23" t="s">
+        <v>195</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>78</v>
@@ -6739,16 +6897,17 @@
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
-        <v>193</v>
+      <c r="A6" s="23" t="s">
+        <v>198</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>78</v>
@@ -6789,16 +6948,17 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
-        <v>196</v>
+      <c r="A7" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>78</v>
@@ -6839,9 +6999,325 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AD144">
+  <conditionalFormatting sqref="A2:AE144">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
@@ -6856,7 +7332,7 @@
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2 M2:O144 K6 A8:L144 P8:AD144">
+  <conditionalFormatting sqref="K2 M2:O144 K6 A8:L144 P8:AE144">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>

</xml_diff>